<commit_message>
Edit phanquyen to be suitable and update db in NGUOIDUNG and HOADON
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\codelearns\wpf\MasterSaveDemo\MasterSaveDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\schoolcode\Nam3\HK1\Baotri\MasterStore\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04928453-05D9-4EB1-8C0B-217F3CD6A447}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9903D108-4C83-4878-8550-A29AE55F2295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="144">
   <si>
     <t>Quản lý nhân sự</t>
   </si>
@@ -97,21 +97,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>ktv1</t>
-  </si>
-  <si>
-    <t>ktv2</t>
-  </si>
-  <si>
-    <t>gdv1</t>
-  </si>
-  <si>
-    <t>gdv2</t>
-  </si>
-  <si>
-    <t>ns1</t>
-  </si>
-  <si>
     <t>QTV_QuanLyNhanSu</t>
   </si>
   <si>
@@ -169,15 +154,6 @@
     <t>Quản Trị Viên</t>
   </si>
   <si>
-    <t>Kiểm Toán Viên</t>
-  </si>
-  <si>
-    <t>Giao Dịch Viên</t>
-  </si>
-  <si>
-    <t>Trưởng Phòng Nhân Sự</t>
-  </si>
-  <si>
     <t>LTK001</t>
   </si>
   <si>
@@ -223,18 +199,6 @@
     <t>Sanh</t>
   </si>
   <si>
-    <t>Tiến</t>
-  </si>
-  <si>
-    <t>Trung</t>
-  </si>
-  <si>
-    <t>Thắng</t>
-  </si>
-  <si>
-    <t>Châu</t>
-  </si>
-  <si>
     <t>STK0000003</t>
   </si>
   <si>
@@ -473,6 +437,39 @@
   </si>
   <si>
     <t>Rút hết</t>
+  </si>
+  <si>
+    <t>Kế Toán Trưởng</t>
+  </si>
+  <si>
+    <t>Thủ Kho</t>
+  </si>
+  <si>
+    <t>Bộ phận Thu ngân</t>
+  </si>
+  <si>
+    <t>ktt1</t>
+  </si>
+  <si>
+    <t>tk1</t>
+  </si>
+  <si>
+    <t>Thảo</t>
+  </si>
+  <si>
+    <t>tn1</t>
+  </si>
+  <si>
+    <t>Hậu</t>
+  </si>
+  <si>
+    <t>Phú Yên</t>
+  </si>
+  <si>
+    <t>Đồng Nai</t>
+  </si>
+  <si>
+    <t>Quảng Nam</t>
   </si>
 </sst>
 </file>
@@ -880,10 +877,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C1" s="3">
         <v>0</v>
@@ -895,18 +892,18 @@
         <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3">
         <v>90</v>
@@ -918,18 +915,18 @@
         <v>90</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3">
         <v>180</v>
@@ -941,10 +938,10 @@
         <v>180</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -956,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
@@ -970,16 +967,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3">
         <v>4500000</v>
@@ -1000,21 +997,21 @@
         <v>4500000</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E2" s="3">
         <v>123456000</v>
@@ -1035,21 +1032,21 @@
         <v>123456000</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3">
         <v>2300000</v>
@@ -1070,21 +1067,21 @@
         <v>2300000</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3">
         <v>1000000</v>
@@ -1105,21 +1102,21 @@
         <v>1000000</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E5" s="3">
         <v>12535000</v>
@@ -1140,24 +1137,24 @@
         <v>12535000</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3">
         <v>12000000</v>
@@ -1178,10 +1175,10 @@
         <v>12000000</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="M6" s="3">
         <v>12010500</v>
@@ -1189,16 +1186,16 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3">
         <v>8500000</v>
@@ -1219,10 +1216,10 @@
         <v>8006493</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="M7" s="3">
         <v>8006604</v>
@@ -1230,16 +1227,16 @@
     </row>
     <row r="8" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E8" s="7">
         <v>50000000</v>
@@ -1260,27 +1257,27 @@
         <v>50000000</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E9" s="7">
         <v>10000000</v>
@@ -1301,27 +1298,27 @@
         <v>9912500</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E10" s="3">
         <v>10000000</v>
@@ -1342,10 +1339,10 @@
         <v>10000000</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M10" s="3">
         <v>10125000</v>
@@ -1353,16 +1350,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E11" s="3">
         <v>15000000</v>
@@ -1383,27 +1380,27 @@
         <v>15000000</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L11" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M11" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3">
         <v>10000000</v>
@@ -1424,10 +1421,10 @@
         <v>10125000</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L12" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="M12" s="3">
         <v>10125140</v>
@@ -1435,16 +1432,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3">
         <v>15000000</v>
@@ -1465,10 +1462,10 @@
         <v>15000000</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L13" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M13" s="3">
         <v>15187500</v>
@@ -1476,16 +1473,16 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E14" s="3">
         <v>5000000</v>
@@ -1506,10 +1503,10 @@
         <v>5000000</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L14" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M14" s="3">
         <v>5137500</v>
@@ -1517,16 +1514,16 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3">
         <v>25000000</v>
@@ -1547,10 +1544,10 @@
         <v>25000000</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L15" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M15" s="3">
         <v>25687500</v>
@@ -1558,16 +1555,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E16" s="3">
         <v>25000000</v>
@@ -1588,27 +1585,27 @@
         <v>25000000</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L16" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M16" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E17" s="3">
         <v>25000000</v>
@@ -1629,10 +1626,10 @@
         <v>25687500</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L17" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="M17" s="3">
         <v>25751005</v>
@@ -1640,16 +1637,16 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E18" s="3">
         <v>5000000</v>
@@ -1670,10 +1667,10 @@
         <v>5137500</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M18" s="3">
         <v>5278781</v>
@@ -1681,16 +1678,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3">
         <v>12000000</v>
@@ -1711,27 +1708,27 @@
         <v>12000000</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="M19" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E20" s="3">
         <v>8500000</v>
@@ -1752,27 +1749,27 @@
         <v>8006493</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L20" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="M20" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E21" s="3">
         <v>50000000</v>
@@ -1793,27 +1790,27 @@
         <v>50000000</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L21" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="M21" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E22" s="3">
         <v>10000000</v>
@@ -1834,27 +1831,27 @@
         <v>9912500</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L22" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="M22" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3">
         <v>10000000</v>
@@ -1875,10 +1872,10 @@
         <v>10000000</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L23" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M23" s="3">
         <v>10125000</v>
@@ -1886,16 +1883,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3">
         <v>15000000</v>
@@ -1916,27 +1913,27 @@
         <v>15000000</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L24" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M24" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E25" s="3">
         <v>10000000</v>
@@ -1957,27 +1954,27 @@
         <v>10125000</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L25" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="M25" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E26" s="3">
         <v>15000000</v>
@@ -1998,10 +1995,10 @@
         <v>15000000</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L26" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M26" s="3">
         <v>15187500</v>
@@ -2009,16 +2006,16 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E27" s="3">
         <v>5000000</v>
@@ -2039,10 +2036,10 @@
         <v>5000000</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L27" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M27" s="3">
         <v>5137500</v>
@@ -2050,16 +2047,16 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E28" s="3">
         <v>25000000</v>
@@ -2080,10 +2077,10 @@
         <v>25000000</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L28" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="M28" s="3">
         <v>25687500</v>
@@ -2091,16 +2088,16 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E29" s="3">
         <v>25000000</v>
@@ -2121,27 +2118,27 @@
         <v>25000000</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L29" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M29" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E30" s="3">
         <v>25000000</v>
@@ -2162,27 +2159,27 @@
         <v>25687500</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L30" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="M30" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E31" s="3">
         <v>5000000</v>
@@ -2203,10 +2200,10 @@
         <v>5137500</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L31" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="M31" s="3">
         <v>5278781</v>
@@ -2238,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C1" s="3">
         <v>1000000</v>
@@ -2249,7 +2246,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C2" s="3">
         <v>100000</v>
@@ -2260,7 +2257,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -2276,7 +2273,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2397,7 +2394,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2420,7 +2417,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2425,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2436,7 +2433,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,7 +2474,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2488,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2499,7 +2496,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2510,7 +2507,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2521,7 +2518,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,7 +2529,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2543,7 +2540,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2554,7 +2551,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2576,7 +2573,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,7 +2584,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2598,7 +2595,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2609,7 +2606,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2620,7 +2617,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2631,7 +2628,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2642,7 +2639,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2653,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2663,103 +2660,112 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37225493-D1D8-4637-A3DD-25B32AA2FDE3}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="12.28515625" style="2"/>
+    <col min="1" max="1" width="12.28515625" style="2"/>
+    <col min="2" max="2" width="8.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2"/>
+    <col min="6" max="6" width="24.42578125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="12.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1">
+        <v>136</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>137</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1">
+        <v>139</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="E4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>